<commit_message>
edit fehrest by imanmdn
</commit_message>
<xml_diff>
--- a/fehrest.xlsx
+++ b/fehrest.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>فصل اول</t>
   </si>
@@ -124,6 +123,87 @@
   </si>
   <si>
     <t>پروژه ی نهایی : هک از طریق Rainbow</t>
+  </si>
+  <si>
+    <t>f1p1</t>
+  </si>
+  <si>
+    <t>f2p2</t>
+  </si>
+  <si>
+    <t>f1p2</t>
+  </si>
+  <si>
+    <t>f1p3</t>
+  </si>
+  <si>
+    <t>f1p4</t>
+  </si>
+  <si>
+    <t>f1p5</t>
+  </si>
+  <si>
+    <t>f1p6</t>
+  </si>
+  <si>
+    <t>f2p1</t>
+  </si>
+  <si>
+    <t>f2p3</t>
+  </si>
+  <si>
+    <t>f2p4</t>
+  </si>
+  <si>
+    <t>f2p5</t>
+  </si>
+  <si>
+    <t>f2p6</t>
+  </si>
+  <si>
+    <t>f3p1</t>
+  </si>
+  <si>
+    <t>f3p2</t>
+  </si>
+  <si>
+    <t>f3p3</t>
+  </si>
+  <si>
+    <t>f3p4</t>
+  </si>
+  <si>
+    <t>f3p5</t>
+  </si>
+  <si>
+    <t>f3p6</t>
+  </si>
+  <si>
+    <t>f3p7</t>
+  </si>
+  <si>
+    <t>f3p8</t>
+  </si>
+  <si>
+    <t>f3p9</t>
+  </si>
+  <si>
+    <t>f3p10</t>
+  </si>
+  <si>
+    <t>f3p11</t>
+  </si>
+  <si>
+    <t>f3p12</t>
+  </si>
+  <si>
+    <t>f4p</t>
+  </si>
+  <si>
+    <t>f5p</t>
+  </si>
+  <si>
+    <t>f6p</t>
   </si>
 </sst>
 </file>
@@ -155,8 +235,9 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="2  Nazanin"/>
-      <charset val="178"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -176,9 +257,15 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -188,16 +275,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -479,214 +578,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection sqref="A1:B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
     <col min="2" max="2" width="55" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A2" s="3"/>
-      <c r="B2" s="5" t="s">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5" t="s">
+    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5" t="s">
+    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5" t="s">
+    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5" t="s">
+    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5" t="s">
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5" t="s">
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5" t="s">
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5" t="s">
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5" t="s">
+    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5" t="s">
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A23" s="3"/>
-      <c r="B23" s="5" t="s">
+    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A24" s="3"/>
-      <c r="B24" s="5" t="s">
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A25" s="3"/>
-      <c r="B25" s="5" t="s">
+    <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A26" s="3"/>
-      <c r="B26" s="5" t="s">
+    <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A27" s="3"/>
-      <c r="B27" s="5" t="s">
+    <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A28" s="3" t="s">
+    <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A29" s="3"/>
-      <c r="B29" s="5" t="s">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A30" s="3" t="s">
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A31" s="3"/>
-      <c r="B31" s="5" t="s">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A32" s="3" t="s">
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7" t="s">
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>